<commit_message>
admin dashboard drop down fix
</commit_message>
<xml_diff>
--- a/work_list.xlsx
+++ b/work_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUF GAMING\Desktop\Training\Smart-Recruiter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E495314-9B37-448B-8D31-E2D5C2B452DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845DBDDD-1614-4A19-940C-D0A8F48CF654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Login page creation</t>
   </si>
@@ -135,7 +135,16 @@
     <t>connection from one interviewer to another interviewer (1st, 2nd, 3rd round connection)</t>
   </si>
   <si>
-    <t>Use set of applicants as one single sission (bundle group of applicants)</t>
+    <t>Use set of applicants as one single session (bundle group of applicants)</t>
+  </si>
+  <si>
+    <t>13/08/ fixes</t>
+  </si>
+  <si>
+    <t>clean the code of candidate storing backend end point (role id should take from query params)</t>
+  </si>
+  <si>
+    <t>admin dashboard dropdown update with job close functionality</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,6 +646,19 @@
         <v>36</v>
       </c>
     </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>